<commit_message>
adds more entries in the metadata sheets
</commit_message>
<xml_diff>
--- a/inst/extdata/metadata-creation-template/example/hannon-example/example-metadata.xlsx
+++ b/inst/extdata/metadata-creation-template/example/hannon-example/example-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Emanuel\Projects\cvpia\EDIutils\inst\extdata\metadata-creation-template\example\hannon-example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6316285D-9383-4689-985E-10E04D923102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79E683F-FF2E-4850-95D5-F18377524685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3270" yWindow="2340" windowWidth="28110" windowHeight="15885" tabRatio="500" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21435" tabRatio="543" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="personnel" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="168">
   <si>
     <t>first_name</t>
   </si>
@@ -538,6 +538,15 @@
   </si>
   <si>
     <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>e-fishing</t>
+  </si>
+  <si>
+    <t>steelhead</t>
+  </si>
+  <si>
+    <t>count of fissh that were naturak predators</t>
   </si>
 </sst>
 </file>
@@ -1014,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1120,7 +1129,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1286,7 +1295,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>165</v>
       </c>
       <c r="B15" t="s">
         <v>123</v>
@@ -1333,7 +1342,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1369,7 +1378,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1412,7 +1421,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1455,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1515,7 +1524,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1549,8 +1558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1620,10 +1629,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1667,6 +1676,11 @@
         <v>67</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1677,7 +1691,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMJ21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3137,12 +3153,30 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>158</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>105</v>
+        <v>167</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>